<commit_message>
added samples to sheets
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_10.02.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_10.02.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1846626-3A18-E445-BB14-540D592000D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02DC88E-B5AE-094F-9839-5CEDFB6AECBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="27">
   <si>
     <t>harvestDate</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>cAMP.20mM</t>
+  </si>
+  <si>
+    <t>cAMP.1.08mM</t>
   </si>
 </sst>
 </file>
@@ -461,13 +464,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -632,7 +638,7 @@
         <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K5">
         <v>30</v>
@@ -667,7 +673,7 @@
         <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K6">
         <v>30</v>
@@ -702,7 +708,7 @@
         <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7">
         <v>30</v>
@@ -737,7 +743,7 @@
         <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8">
         <v>30</v>
@@ -772,7 +778,7 @@
         <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9">
         <v>30</v>
@@ -807,10 +813,10 @@
         <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K10">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -842,7 +848,7 @@
         <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K11">
         <v>90</v>
@@ -877,7 +883,7 @@
         <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K12">
         <v>90</v>
@@ -912,7 +918,7 @@
         <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K13">
         <v>90</v>
@@ -947,7 +953,7 @@
         <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K14">
         <v>90</v>
@@ -982,7 +988,7 @@
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K15">
         <v>90</v>
@@ -1017,10 +1023,10 @@
         <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K16">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="L16">
         <v>2</v>
@@ -1052,10 +1058,10 @@
         <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K17">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="L17">
         <v>2</v>
@@ -1087,7 +1093,7 @@
         <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K18">
         <v>180</v>
@@ -1122,7 +1128,7 @@
         <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K19">
         <v>180</v>
@@ -1157,7 +1163,7 @@
         <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K20">
         <v>180</v>
@@ -1192,7 +1198,7 @@
         <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K21">
         <v>180</v>
@@ -1227,10 +1233,10 @@
         <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K22">
-        <v>1440</v>
+        <v>180</v>
       </c>
       <c r="L22">
         <v>2</v>
@@ -1262,10 +1268,10 @@
         <v>19</v>
       </c>
       <c r="J23" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K23">
-        <v>1440</v>
+        <v>180</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -1297,10 +1303,10 @@
         <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K24">
-        <v>1440</v>
+        <v>180</v>
       </c>
       <c r="L24">
         <v>2</v>
@@ -1332,7 +1338,7 @@
         <v>19</v>
       </c>
       <c r="J25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K25">
         <v>1440</v>
@@ -1367,7 +1373,7 @@
         <v>19</v>
       </c>
       <c r="J26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K26">
         <v>1440</v>
@@ -1402,12 +1408,152 @@
         <v>19</v>
       </c>
       <c r="J27" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K27">
         <v>1440</v>
       </c>
       <c r="L27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28">
+        <v>1440</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29">
+        <v>1440</v>
+      </c>
+      <c r="L29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" t="s">
+        <v>24</v>
+      </c>
+      <c r="K30">
+        <v>1440</v>
+      </c>
+      <c r="L30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31">
+        <v>1440</v>
+      </c>
+      <c r="L31">
         <v>2</v>
       </c>
     </row>

</xml_diff>